<commit_message>
ver_0.12 item 구매 구현. MessageBox는 coroutine 사용
</commit_message>
<xml_diff>
--- a/창의적종합설계 신청서/재료비 구매리스트.xlsx
+++ b/창의적종합설계 신청서/재료비 구매리스트.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gyuho\OneDrive - 경희대학교\바탕 화면\3. 창의적종합설계\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\82105\OneDrive - 경희대학교\바탕 화면\RV\창의적종합설계 신청서\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="27876" windowHeight="12840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
   </bookViews>
   <sheets>
     <sheet name="팀명" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>합계</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -80,53 +80,97 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Vuforia classic ver</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AR Engine</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Web</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.ptc.com/</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>12 Augmented Reality apps with Unity &amp; Vuforia</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vuforia Lecture</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Web</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.udemy.com/</t>
-  </si>
-  <si>
-    <t>https://www.udemy.com/</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NLP Practitioner Certificate Cource</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NLP Lecture</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>라즈베리파이3 B+ 터치스크린 7인치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>라즈베리파이3 B+ 터치스크린 케이스</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>삼성 Micro SD 카드 256GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB Micro SD Reader</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDMI 케이블</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LAN 케이블</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.devicemart.co.kr/goods/view?no=1273487</t>
+  </si>
+  <si>
+    <t>https://www.devicemart.co.kr/goods/view?no=1312315</t>
+  </si>
+  <si>
+    <t>https://www.devicemart.co.kr/goods/view?no=10830717</t>
+  </si>
+  <si>
+    <t>https://www.devicemart.co.kr/goods/view?no=1232573</t>
+  </si>
+  <si>
+    <t>https://www.icbanq.com/P008271082</t>
+  </si>
+  <si>
+    <t>라즈베리파이3 B+ 본체, 어댑터, 방열판</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>라즈베리파이3 B+ 듀얼쿨링팬 + 방열케이스</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.icbanq.com/P008890303</t>
+  </si>
+  <si>
+    <t>https://www.icbanq.com/P007447297</t>
+  </si>
+  <si>
+    <t>https://www.icbanq.com/P008936201</t>
+  </si>
+  <si>
+    <t>키보드, 마우스 세트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://dongyangtool.com/detail.php?pt_idx=1060032&amp;NaPm=ct%3Djw76zsyo%7Cci%3D56ee44039777c08683b38ea0e21a7ed1d4e6efd9%7Ctr%3Dslsl%7Csn%3D931938%7Chk%3Dca92cfcf6449015bd1fca4467436ba3c9b5e4d8f</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -334,7 +378,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -353,9 +397,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -392,19 +433,25 @@
     <xf numFmtId="41" fontId="10" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -417,21 +464,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -722,8 +754,8 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -739,436 +771,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="20" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="E6" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="21">
+        <v>48000</v>
+      </c>
+      <c r="G6" s="17">
+        <v>3</v>
+      </c>
+      <c r="H6" s="14">
+        <f>F6*G6</f>
+        <v>144000</v>
+      </c>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="13">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="22">
+        <v>15000</v>
+      </c>
+      <c r="G7" s="18">
+        <v>3</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" ref="H7" si="0">F7*G7</f>
+        <v>45000</v>
+      </c>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="13">
+        <v>3</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="29" t="s">
+      <c r="E8" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="22">
+        <v>86500</v>
+      </c>
+      <c r="G8" s="18">
+        <v>3</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" ref="H8:H14" si="1">F8*G8</f>
+        <v>259500</v>
+      </c>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="13">
+        <v>4</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="30">
-        <v>580000</v>
-      </c>
-      <c r="G6" s="18">
-        <v>1</v>
-      </c>
-      <c r="H6" s="15">
-        <f>F6*G6</f>
-        <v>580000</v>
-      </c>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="22">
+        <v>31000</v>
+      </c>
+      <c r="G9" s="18">
+        <v>3</v>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="1"/>
+        <v>93000</v>
+      </c>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="9">
+        <v>5</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="24">
+        <v>7700</v>
+      </c>
+      <c r="G10" s="19">
+        <v>3</v>
+      </c>
+      <c r="H10" s="14">
+        <f t="shared" ref="H10:H11" si="2">F10*G10</f>
+        <v>23100</v>
+      </c>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="9">
+        <v>6</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="22">
+        <v>3000</v>
+      </c>
+      <c r="G11" s="18">
+        <v>3</v>
+      </c>
+      <c r="H11" s="14">
+        <f t="shared" si="2"/>
+        <v>9000</v>
+      </c>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="9">
+        <v>7</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="22">
+        <v>46800</v>
+      </c>
+      <c r="G12" s="18">
+        <v>3</v>
+      </c>
+      <c r="H12" s="14">
+        <f t="shared" si="1"/>
+        <v>140400</v>
+      </c>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="11">
+        <v>8</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="22">
+        <v>6000</v>
+      </c>
+      <c r="G13" s="18">
         <v>2</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="32">
-        <v>13000</v>
-      </c>
-      <c r="G7" s="20">
-        <v>1</v>
-      </c>
-      <c r="H7" s="15">
-        <f t="shared" ref="H7:H16" si="0">F7*G7</f>
-        <v>13000</v>
-      </c>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="14">
-        <v>3</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="14" t="s">
+      <c r="H13" s="14">
+        <f t="shared" ref="H13" si="3">F13*G13</f>
+        <v>12000</v>
+      </c>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="9">
+        <v>9</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="32">
-        <v>13000</v>
-      </c>
-      <c r="G8" s="20">
-        <v>1</v>
-      </c>
-      <c r="H8" s="15">
-        <f t="shared" si="0"/>
-        <v>13000</v>
-      </c>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="14">
-        <v>4</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="15">
-        <f t="shared" si="0"/>
+      <c r="E14" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="22">
+        <v>10000</v>
+      </c>
+      <c r="G14" s="18">
+        <v>2</v>
+      </c>
+      <c r="H14" s="14">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="10">
-        <v>5</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="10">
-        <v>6</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="10">
-        <v>7</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="10">
-        <v>8</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="10">
-        <v>9</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="10">
-        <v>10</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="3">
+        <f>SUM(F6:F14)</f>
+        <v>254000</v>
+      </c>
+      <c r="G15" s="3">
+        <f>SUM(G6:G14)</f>
+        <v>25</v>
+      </c>
+      <c r="H15" s="3">
+        <f>SUM(H6:H14)</f>
+        <v>746000</v>
       </c>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="10">
-        <v>11</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="10">
-        <v>12</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+    <row r="17" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="10">
-        <v>13</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+    <row r="18" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="10">
-        <v>14</v>
-      </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+    <row r="19" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="10">
-        <v>15</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+    <row r="20" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="10">
-        <v>16</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+    <row r="21" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="10">
-        <v>17</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+    <row r="22" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="10">
-        <v>18</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+    <row r="23" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="10">
-        <v>19</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+    <row r="24" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="10">
-        <v>20</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+    <row r="25" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="26"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3">
-        <f>SUM(F6:F25)</f>
-        <v>606000</v>
-      </c>
-      <c r="G26" s="3">
-        <f>SUM(G6:G25)</f>
-        <v>3</v>
-      </c>
-      <c r="H26" s="3">
-        <f>SUM(H6:H25)</f>
-        <v>606000</v>
-      </c>
+    <row r="26" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="9:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E7" r:id="rId2"/>
-    <hyperlink ref="E8" r:id="rId3"/>
+    <hyperlink ref="E8" r:id="rId1"/>
+    <hyperlink ref="E9" r:id="rId2"/>
+    <hyperlink ref="E12" r:id="rId3"/>
+    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E10" r:id="rId6"/>
+    <hyperlink ref="E11" r:id="rId7"/>
+    <hyperlink ref="E13" r:id="rId8"/>
+    <hyperlink ref="E14" r:id="rId9"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ver 0.13 target change(beer can)
</commit_message>
<xml_diff>
--- a/창의적종합설계 신청서/재료비 구매리스트.xlsx
+++ b/창의적종합설계 신청서/재료비 구매리스트.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9108"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="팀명" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>합계</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -68,18 +74,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>굇.수</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>권형진</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>01035198164</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Web</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -165,6 +159,33 @@
   </si>
   <si>
     <t>http://dongyangtool.com/detail.php?pt_idx=1060032&amp;NaPm=ct%3Djw76zsyo%7Cci%3D56ee44039777c08683b38ea0e21a7ed1d4e6efd9%7Ctr%3Dslsl%7Csn%3D931938%7Chk%3Dca92cfcf6449015bd1fca4467436ba3c9b5e4d8f</t>
+  </si>
+  <si>
+    <t>Web</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.nxp.com/products/processors-and-microcontrollers/arm-based-processors-and-mcus/i.mx-applications-processors/i.mx-8-processors/coral-dev-board-tpu:CORAL-EDGE-TPU</t>
+  </si>
+  <si>
+    <t>Coral TPU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이규호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>010-5721-0601</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>굇.수 -&gt; 해커(Hacker)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>어플리케이션 서버, DataBase 저장용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -752,10 +773,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -763,7 +784,7 @@
     <col min="1" max="1" width="4.69921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.09765625" customWidth="1"/>
     <col min="3" max="4" width="21.3984375" customWidth="1"/>
-    <col min="5" max="5" width="43.3984375" customWidth="1"/>
+    <col min="5" max="5" width="202.296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
     <col min="8" max="8" width="12.59765625" style="1" customWidth="1"/>
@@ -772,7 +793,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="25.2" x14ac:dyDescent="0.4">
       <c r="A1" s="25" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
@@ -788,7 +809,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.4">
@@ -796,7 +817,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -841,14 +862,14 @@
         <v>1</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F6" s="21">
         <v>48000</v>
@@ -860,21 +881,23 @@
         <f>F6*G6</f>
         <v>144000</v>
       </c>
-      <c r="I6" s="13"/>
+      <c r="I6" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="13">
         <v>2</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F7" s="22">
         <v>15000</v>
@@ -886,21 +909,23 @@
         <f t="shared" ref="H7" si="0">F7*G7</f>
         <v>45000</v>
       </c>
-      <c r="I7" s="13"/>
+      <c r="I7" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="13">
         <v>3</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F8" s="22">
         <v>86500</v>
@@ -909,24 +934,26 @@
         <v>3</v>
       </c>
       <c r="H8" s="14">
-        <f t="shared" ref="H8:H14" si="1">F8*G8</f>
+        <f t="shared" ref="H8:H15" si="1">F8*G8</f>
         <v>259500</v>
       </c>
-      <c r="I8" s="13"/>
+      <c r="I8" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="13">
         <v>4</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F9" s="22">
         <v>31000</v>
@@ -938,21 +965,23 @@
         <f t="shared" si="1"/>
         <v>93000</v>
       </c>
-      <c r="I9" s="13"/>
+      <c r="I9" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="9">
         <v>5</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" s="24">
         <v>7700</v>
@@ -964,21 +993,23 @@
         <f t="shared" ref="H10:H11" si="2">F10*G10</f>
         <v>23100</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="9">
         <v>6</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F11" s="22">
         <v>3000</v>
@@ -990,21 +1021,23 @@
         <f t="shared" si="2"/>
         <v>9000</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="9">
         <v>7</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F12" s="22">
         <v>46800</v>
@@ -1016,21 +1049,23 @@
         <f t="shared" si="1"/>
         <v>140400</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11">
         <v>8</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F13" s="22">
         <v>6000</v>
@@ -1042,57 +1077,85 @@
         <f t="shared" ref="H13" si="3">F13*G13</f>
         <v>12000</v>
       </c>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="9">
+      <c r="I13" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="11">
         <v>9</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="13" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="22">
+        <v>180000</v>
+      </c>
+      <c r="G14" s="18">
+        <v>1</v>
+      </c>
+      <c r="H14" s="14">
+        <v>180000</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="9">
+        <v>9</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="22">
         <v>10000</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G15" s="18">
         <v>2</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H15" s="14">
         <f t="shared" si="1"/>
         <v>20000</v>
       </c>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="26" t="s">
+      <c r="I15" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="3">
-        <f>SUM(F6:F14)</f>
-        <v>254000</v>
-      </c>
-      <c r="G15" s="3">
-        <f>SUM(G6:G14)</f>
-        <v>25</v>
-      </c>
-      <c r="H15" s="3">
-        <f>SUM(H6:H14)</f>
-        <v>746000</v>
-      </c>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="3">
+        <f>SUM(F6:F15)</f>
+        <v>434000</v>
+      </c>
+      <c r="G16" s="3">
+        <f>SUM(G6:G15)</f>
+        <v>26</v>
+      </c>
+      <c r="H16" s="3">
+        <f>SUM(H6:H15)</f>
+        <v>926000</v>
+      </c>
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
@@ -1123,13 +1186,16 @@
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="9:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.4"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="9:9" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="9:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1141,10 +1207,11 @@
     <hyperlink ref="E10" r:id="rId6"/>
     <hyperlink ref="E11" r:id="rId7"/>
     <hyperlink ref="E13" r:id="rId8"/>
-    <hyperlink ref="E14" r:id="rId9"/>
+    <hyperlink ref="E15" r:id="rId9"/>
+    <hyperlink ref="E14" r:id="rId10"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId10"/>
+  <pageSetup paperSize="9" scale="85" orientation="landscape" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>